<commit_message>
Add every update accur
</commit_message>
<xml_diff>
--- a/Assignment2/Report/report.xlsx
+++ b/Assignment2/Report/report.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\OSU CS\MachineLearning\Assignment2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\OSU CS\MachineLearning\Assignment2\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
     <sheet name="apha15" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">GenPerceptron!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">GenPerceptron!$A$1:$E$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="6">
   <si>
     <t>Training Data</t>
   </si>
@@ -41,16 +41,16 @@
     <t>Validate Data</t>
   </si>
   <si>
-    <t>0.9656301145662848          0.9459791282995703</t>
+    <t>did not achieve 100%, maybe because last update weight</t>
   </si>
   <si>
-    <t>0.954582651391162           0.9404542664211173</t>
+    <t>JerryTrain</t>
   </si>
   <si>
-    <t>最後兩筆怪怪的, should be same result as online perceptron</t>
+    <t>最後兩筆怪怪的, should be same as online perceptron result</t>
   </si>
   <si>
-    <t>did not achieve 100%, maybe because last update weight</t>
+    <t>JerryTraining</t>
   </si>
 </sst>
 </file>
@@ -130,7 +130,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>GenPerceptron!$B$1</c:f>
+              <c:f>GenPerceptron!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -153,7 +153,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>GenPerceptron!$B$2:$B$16</c:f>
+              <c:f>GenPerceptron!$C$2:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -212,7 +212,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>GenPerceptron!$C$1</c:f>
+              <c:f>GenPerceptron!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -235,7 +235,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>GenPerceptron!$C$2:$C$16</c:f>
+              <c:f>GenPerceptron!$D$2:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -283,6 +283,88 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0.94597912829956998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>GenPerceptron!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>JerryTraining</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>GenPerceptron!$B$2:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.90773322422258595</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.93617021276595702</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.93821603927986896</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.94476268412438602</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.948240589198036</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.948445171849427</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.94905891980360002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.94905891980360002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.95110474631751196</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.95171849427168498</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.95192307692307598</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.95560556464811697</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.95355973813420603</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.95560556464811697</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.95478723404255295</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -298,11 +380,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1509225168"/>
-        <c:axId val="-1509219184"/>
+        <c:axId val="-705482720"/>
+        <c:axId val="-705478912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1509225168"/>
+        <c:axId val="-705482720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -345,7 +427,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1509219184"/>
+        <c:crossAx val="-705478912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -353,7 +435,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1509219184"/>
+        <c:axId val="-705478912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -404,7 +486,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1509225168"/>
+        <c:crossAx val="-705482720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -510,7 +592,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>AvgPercepron!$B$1</c:f>
+              <c:f>AvgPercepron!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -533,7 +615,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>AvgPercepron!$B$2:$B$16</c:f>
+              <c:f>AvgPercepron!$C$2:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -592,7 +674,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>AvgPercepron!$C$1</c:f>
+              <c:f>AvgPercepron!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -615,7 +697,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>AvgPercepron!$C$2:$C$16</c:f>
+              <c:f>AvgPercepron!$D$2:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -663,6 +745,88 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0.95395948434622402</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>AvgPercepron!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>JerryTraining</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>AvgPercepron!$B$2:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.90773322422258595</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.93617021276595702</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.93821603927986896</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.94476268412438602</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.948240589198036</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.948445171849427</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.94905891980360002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.94905891980360002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.95110474631751196</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.95171849427168498</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.95192307692307598</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.95560556464811697</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.95355973813420603</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.95560556464811697</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.95478723404255295</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -678,11 +842,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1509224624"/>
-        <c:axId val="-1509220816"/>
+        <c:axId val="-705477280"/>
+        <c:axId val="-816066816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1509224624"/>
+        <c:axId val="-705477280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -725,7 +889,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1509220816"/>
+        <c:crossAx val="-816066816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -733,7 +897,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1509220816"/>
+        <c:axId val="-816066816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -784,7 +948,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1509224624"/>
+        <c:crossAx val="-705477280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -890,7 +1054,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>apha1!$B$1</c:f>
+              <c:f>apha1!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -967,7 +1131,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>apha1!$B$2:$B$16</c:f>
+              <c:f>apha1!$C$2:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1011,10 +1175,10 @@
                   <c:v>0.96460720130932898</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.96624386252045802</c:v>
+                  <c:v>0.965630114566284</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.95642389525368199</c:v>
+                  <c:v>0.95458265139116205</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1026,7 +1190,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>apha1!$C$1</c:f>
+              <c:f>apha1!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1103,7 +1267,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>apha1!$C$2:$C$16</c:f>
+              <c:f>apha1!$D$2:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1147,10 +1311,92 @@
                   <c:v>0.94229588704726797</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.95273173726212401</c:v>
+                  <c:v>0.94597912829956998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.94597912829956998</c:v>
+                  <c:v>0.94045426642111696</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>apha1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>JerryTrain</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>apha1!$B$2:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.90773322422258595</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.93617021276595702</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.93821603927986896</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.94476268412438602</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.948240589198036</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.948445171849427</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.94905891980360002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.94905891980360002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.95110474631751196</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.95171849427168498</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.95192307692307598</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.95560556464811697</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.95355973813420603</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.95662847790507299</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.95130932896890297</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1166,11 +1412,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1404813584"/>
-        <c:axId val="-1404820656"/>
+        <c:axId val="-816066272"/>
+        <c:axId val="-566167152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1404813584"/>
+        <c:axId val="-816066272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1213,7 +1459,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1404820656"/>
+        <c:crossAx val="-566167152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1221,7 +1467,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1404820656"/>
+        <c:axId val="-566167152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1272,7 +1518,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1404813584"/>
+        <c:crossAx val="-816066272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1378,7 +1624,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>apha2!$B$1</c:f>
+              <c:f>apha2!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1455,7 +1701,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>apha2!$B$2:$B$16</c:f>
+              <c:f>apha2!$C$2:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1514,7 +1760,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>apha2!$C$1</c:f>
+              <c:f>apha2!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1591,7 +1837,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>apha2!$C$2:$C$16</c:f>
+              <c:f>apha2!$D$2:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1640,6 +1886,43 @@
                 <c:pt idx="14">
                   <c:v>0.97237569060773399</c:v>
                 </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>apha2!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>JerryTraining</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>apha2!$B$2:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1654,11 +1937,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1509218096"/>
-        <c:axId val="-1509214832"/>
+        <c:axId val="-566169328"/>
+        <c:axId val="-566174768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1509218096"/>
+        <c:axId val="-566169328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1701,7 +1984,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1509214832"/>
+        <c:crossAx val="-566174768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1709,7 +1992,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1509214832"/>
+        <c:axId val="-566174768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1760,7 +2043,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1509218096"/>
+        <c:crossAx val="-566169328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1866,7 +2149,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>apha3!$B$1</c:f>
+              <c:f>apha3!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1943,7 +2226,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>apha3!$B$2:$B$16</c:f>
+              <c:f>apha3!$C$2:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -2002,7 +2285,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>apha3!$C$1</c:f>
+              <c:f>apha3!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2079,7 +2362,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>apha3!$C$2:$C$16</c:f>
+              <c:f>apha3!$D$2:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -2128,6 +2411,43 @@
                 <c:pt idx="14">
                   <c:v>0.98281154082259004</c:v>
                 </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>apha3!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>JerryTraining</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>apha3!$B$2:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2142,11 +2462,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1509214288"/>
-        <c:axId val="-1509221904"/>
+        <c:axId val="-566170416"/>
+        <c:axId val="-566179120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1509214288"/>
+        <c:axId val="-566170416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2189,7 +2509,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1509221904"/>
+        <c:crossAx val="-566179120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2197,7 +2517,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1509221904"/>
+        <c:axId val="-566179120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2248,7 +2568,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1509214288"/>
+        <c:crossAx val="-566170416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2354,7 +2674,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>apha7!$B$1</c:f>
+              <c:f>apha7!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2431,7 +2751,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>apha7!$B$2:$B$16</c:f>
+              <c:f>apha7!$C$2:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -2490,7 +2810,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>apha7!$C$1</c:f>
+              <c:f>apha7!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2567,7 +2887,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>apha7!$C$2:$C$16</c:f>
+              <c:f>apha7!$D$2:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -2616,6 +2936,43 @@
                 <c:pt idx="14">
                   <c:v>0.97728667894413701</c:v>
                 </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>apha7!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>JerryTraining</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>apha7!$B$2:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2630,11 +2987,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1509213200"/>
-        <c:axId val="-1509226256"/>
+        <c:axId val="-566181840"/>
+        <c:axId val="-566180208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1509213200"/>
+        <c:axId val="-566181840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2677,7 +3034,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1509226256"/>
+        <c:crossAx val="-566180208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2685,7 +3042,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1509226256"/>
+        <c:axId val="-566180208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2736,7 +3093,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1509213200"/>
+        <c:crossAx val="-566181840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2842,7 +3199,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>apha15!$B$1</c:f>
+              <c:f>apha15!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2919,7 +3276,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>apha15!$B$2:$B$16</c:f>
+              <c:f>apha15!$C$2:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -2978,7 +3335,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>apha15!$C$1</c:f>
+              <c:f>apha15!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3055,7 +3412,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>apha15!$C$2:$C$16</c:f>
+              <c:f>apha15!$D$2:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -3104,6 +3461,43 @@
                 <c:pt idx="14">
                   <c:v>0.96562308164518096</c:v>
                 </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>apha15!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>JerryTraining</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>apha15!$B$2:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3118,11 +3512,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1687811760"/>
-        <c:axId val="-1687810672"/>
+        <c:axId val="-566179664"/>
+        <c:axId val="-566173136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1687811760"/>
+        <c:axId val="-566179664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3165,7 +3559,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1687810672"/>
+        <c:crossAx val="-566173136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3173,7 +3567,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1687810672"/>
+        <c:axId val="-566173136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3224,7 +3618,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1687811760"/>
+        <c:crossAx val="-566179664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7201,13 +7595,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>555625</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>3175</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>250825</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>168275</xdr:rowOff>
@@ -7236,13 +7630,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>368300</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>79375</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>63500</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>60325</xdr:rowOff>
@@ -7271,13 +7665,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>50800</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>79375</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>355600</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>60325</xdr:rowOff>
@@ -7306,13 +7700,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>400050</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>174625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>155575</xdr:rowOff>
@@ -7341,13 +7735,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>501650</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>149225</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>196850</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>130175</xdr:rowOff>
@@ -7376,13 +7770,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>50800</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>355600</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
@@ -7411,13 +7805,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
@@ -7705,252 +8099,301 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
+        <v>0.90773322422258595</v>
+      </c>
+      <c r="C2">
         <v>0.94742225859247098</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>0.93370165745856304</v>
       </c>
-      <c r="D2">
-        <f>B2-C2</f>
+      <c r="E2">
+        <f t="shared" ref="E2:E16" si="0">C2-D2</f>
         <v>1.3720601133907939E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
+        <v>0.93617021276595702</v>
+      </c>
+      <c r="C3">
         <v>0.95765139116202902</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>0.94536525475751998</v>
       </c>
-      <c r="D3">
-        <f>B3-C3</f>
+      <c r="E3">
+        <f t="shared" si="0"/>
         <v>1.228613640450904E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
+        <v>0.93821603927986896</v>
+      </c>
+      <c r="C4">
         <v>0.94987725040916504</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>0.93492940454266404</v>
       </c>
-      <c r="D4">
-        <f>B4-C4</f>
+      <c r="E4">
+        <f t="shared" si="0"/>
         <v>1.4947845866500997E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
+        <v>0.94476268412438602</v>
+      </c>
+      <c r="C5">
         <v>0.96481178396071998</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>0.94843462246777099</v>
       </c>
-      <c r="D5">
-        <f>B5-C5</f>
+      <c r="E5">
+        <f t="shared" si="0"/>
         <v>1.6377161492948988E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
+        <v>0.948240589198036</v>
+      </c>
+      <c r="C6">
         <v>0.956833060556464</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>0.93677102516881505</v>
       </c>
-      <c r="D6">
-        <f>B6-C6</f>
+      <c r="E6">
+        <f t="shared" si="0"/>
         <v>2.0062035387648947E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
+        <v>0.948445171849427</v>
+      </c>
+      <c r="C7">
         <v>0.95765139116202902</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>0.94352363413136897</v>
       </c>
-      <c r="D7">
-        <f>B7-C7</f>
+      <c r="E7">
+        <f t="shared" si="0"/>
         <v>1.4127757030660049E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
+        <v>0.94905891980360002</v>
+      </c>
+      <c r="C8">
         <v>0.95887888707037605</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>0.93799877225291595</v>
       </c>
-      <c r="D8">
-        <f>B8-C8</f>
+      <c r="E8">
+        <f t="shared" si="0"/>
         <v>2.0880114817460105E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
+        <v>0.94905891980360002</v>
+      </c>
+      <c r="C9">
         <v>0.95662847790507299</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>0.93861264579496595</v>
       </c>
-      <c r="D9">
-        <f>B9-C9</f>
+      <c r="E9">
+        <f t="shared" si="0"/>
         <v>1.8015832110107044E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
+        <v>0.95110474631751196</v>
+      </c>
+      <c r="C10">
         <v>0.95908346972176695</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>0.94782074892572099</v>
       </c>
-      <c r="D10">
-        <f>B10-C10</f>
+      <c r="E10">
+        <f t="shared" si="0"/>
         <v>1.1262720796045955E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
+        <v>0.95171849427168498</v>
+      </c>
+      <c r="C11">
         <v>0.96215220949263502</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>0.93922651933701595</v>
       </c>
-      <c r="D11">
-        <f>B11-C11</f>
+      <c r="E11">
+        <f t="shared" si="0"/>
         <v>2.2925690155619072E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
+        <v>0.95192307692307598</v>
+      </c>
+      <c r="C12">
         <v>0.96215220949263502</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>0.94045426642111696</v>
       </c>
-      <c r="D12">
-        <f>B12-C12</f>
+      <c r="E12">
+        <f t="shared" si="0"/>
         <v>2.1697943071518067E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
+        <v>0.95560556464811697</v>
+      </c>
+      <c r="C13">
         <v>0.95908346972176695</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>0.94290976058931797</v>
       </c>
-      <c r="D13">
-        <f>B13-C13</f>
+      <c r="E13">
+        <f t="shared" si="0"/>
         <v>1.6173709132448977E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
+        <v>0.95355973813420603</v>
+      </c>
+      <c r="C14">
         <v>0.96460720130932898</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>0.94229588704726797</v>
       </c>
-      <c r="D14">
-        <f>B14-C14</f>
+      <c r="E14">
+        <f t="shared" si="0"/>
         <v>2.2311314262061011E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
+        <v>0.95560556464811697</v>
+      </c>
+      <c r="C15">
         <v>0.96624386252045802</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>0.95273173726212401</v>
       </c>
-      <c r="D15">
-        <f>B15-C15</f>
+      <c r="E15">
+        <f t="shared" si="0"/>
         <v>1.3512125258334007E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
+        <v>0.95478723404255295</v>
+      </c>
+      <c r="C16">
         <v>0.95642389525368199</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>0.94597912829956998</v>
       </c>
-      <c r="D16">
-        <f>B16-C16</f>
+      <c r="E16">
+        <f t="shared" si="0"/>
         <v>1.0444766954112006E-2</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1"/>
+  <autoFilter ref="A1:E1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -7958,248 +8401,297 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D1048576"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="3" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
+        <v>0.90773322422258595</v>
+      </c>
+      <c r="C2">
         <v>0.95642389525368199</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>0.94475138121546898</v>
       </c>
-      <c r="D2">
-        <f>B2-C2</f>
+      <c r="E2">
+        <f t="shared" ref="E2:E16" si="0">C2-D2</f>
         <v>1.1672514038213011E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
+        <v>0.93617021276595702</v>
+      </c>
+      <c r="C3">
         <v>0.96174304418985201</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>0.949662369551872</v>
       </c>
-      <c r="D3">
-        <f>B3-C3</f>
+      <c r="E3">
+        <f t="shared" si="0"/>
         <v>1.2080674637980016E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
+        <v>0.93821603927986896</v>
+      </c>
+      <c r="C4">
         <v>0.96297054009819905</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>0.95150399017802301</v>
       </c>
-      <c r="D4">
-        <f>B4-C4</f>
+      <c r="E4">
+        <f t="shared" si="0"/>
         <v>1.1466549920176039E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
+        <v>0.94476268412438602</v>
+      </c>
+      <c r="C5">
         <v>0.96624386252045802</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>0.950890116635973</v>
       </c>
-      <c r="D5">
-        <f>B5-C5</f>
+      <c r="E5">
+        <f t="shared" si="0"/>
         <v>1.5353745884485015E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
+        <v>0.948240589198036</v>
+      </c>
+      <c r="C6">
         <v>0.96767594108019594</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>0.950276243093922</v>
       </c>
-      <c r="D6">
-        <f>B6-C6</f>
+      <c r="E6">
+        <f t="shared" si="0"/>
         <v>1.7399697986273943E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
+        <v>0.948445171849427</v>
+      </c>
+      <c r="C7">
         <v>0.96706219312602204</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>0.950890116635973</v>
       </c>
-      <c r="D7">
-        <f>B7-C7</f>
+      <c r="E7">
+        <f t="shared" si="0"/>
         <v>1.6172076490049037E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
+        <v>0.94905891980360002</v>
+      </c>
+      <c r="C8">
         <v>0.96828968903436896</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>0.95150399017802301</v>
       </c>
-      <c r="D8">
-        <f>B8-C8</f>
+      <c r="E8">
+        <f t="shared" si="0"/>
         <v>1.6785698856345954E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
+        <v>0.94905891980360002</v>
+      </c>
+      <c r="C9">
         <v>0.96849427168576097</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>0.95273173726212401</v>
       </c>
-      <c r="D9">
-        <f>B9-C9</f>
+      <c r="E9">
+        <f t="shared" si="0"/>
         <v>1.5762534423636954E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
+        <v>0.95110474631751196</v>
+      </c>
+      <c r="C10">
         <v>0.96890343698854298</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>0.95211786372007301</v>
       </c>
-      <c r="D10">
-        <f>B10-C10</f>
+      <c r="E10">
+        <f t="shared" si="0"/>
         <v>1.6785573268469967E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
+        <v>0.95171849427168498</v>
+      </c>
+      <c r="C11">
         <v>0.96890343698854298</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>0.95273173726212401</v>
       </c>
-      <c r="D11">
-        <f>B11-C11</f>
+      <c r="E11">
+        <f t="shared" si="0"/>
         <v>1.6171699726418964E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
+        <v>0.95192307692307598</v>
+      </c>
+      <c r="C12">
         <v>0.969721767594108</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>0.95273173726212401</v>
       </c>
-      <c r="D12">
-        <f>B12-C12</f>
+      <c r="E12">
+        <f t="shared" si="0"/>
         <v>1.6990030331983985E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
+        <v>0.95560556464811697</v>
+      </c>
+      <c r="C13">
         <v>0.97013093289689001</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>0.95273173726212401</v>
       </c>
-      <c r="D13">
-        <f>B13-C13</f>
+      <c r="E13">
+        <f t="shared" si="0"/>
         <v>1.7399195634765996E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
+        <v>0.95355973813420603</v>
+      </c>
+      <c r="C14">
         <v>0.97074468085106302</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>0.95273173726212401</v>
       </c>
-      <c r="D14">
-        <f>B14-C14</f>
+      <c r="E14">
+        <f t="shared" si="0"/>
         <v>1.8012943588939012E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
+        <v>0.95560556464811697</v>
+      </c>
+      <c r="C15">
         <v>0.97054009819967202</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>0.95273173726212401</v>
       </c>
-      <c r="D15">
-        <f>B15-C15</f>
+      <c r="E15">
+        <f t="shared" si="0"/>
         <v>1.7808360937548007E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
+        <v>0.95478723404255295</v>
+      </c>
+      <c r="C16">
         <v>0.97094926350245503</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>0.95395948434622402</v>
       </c>
-      <c r="D16">
-        <f>B16-C16</f>
+      <c r="E16">
+        <f t="shared" si="0"/>
         <v>1.6989779156231011E-2</v>
       </c>
     </row>
@@ -8211,264 +8703,303 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="3" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
+        <v>0.90773322422258595</v>
+      </c>
+      <c r="C2">
         <v>0.94742225859247098</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>0.93370165745856304</v>
       </c>
-      <c r="D2">
-        <f>B2-C2</f>
+      <c r="E2">
+        <f t="shared" ref="E2:E16" si="0">C2-D2</f>
         <v>1.3720601133907939E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
+        <v>0.93617021276595702</v>
+      </c>
+      <c r="C3">
         <v>0.95765139116202902</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>0.94536525475751998</v>
       </c>
-      <c r="D3">
-        <f>B3-C3</f>
+      <c r="E3">
+        <f t="shared" si="0"/>
         <v>1.228613640450904E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
+        <v>0.93821603927986896</v>
+      </c>
+      <c r="C4">
         <v>0.94987725040916504</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>0.93492940454266404</v>
       </c>
-      <c r="D4">
-        <f>B4-C4</f>
+      <c r="E4">
+        <f t="shared" si="0"/>
         <v>1.4947845866500997E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
+        <v>0.94476268412438602</v>
+      </c>
+      <c r="C5">
         <v>0.96481178396071998</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>0.94843462246777099</v>
       </c>
-      <c r="D5">
-        <f>B5-C5</f>
+      <c r="E5">
+        <f t="shared" si="0"/>
         <v>1.6377161492948988E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
+        <v>0.948240589198036</v>
+      </c>
+      <c r="C6">
         <v>0.956833060556464</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>0.93677102516881505</v>
       </c>
-      <c r="D6">
-        <f>B6-C6</f>
+      <c r="E6">
+        <f t="shared" si="0"/>
         <v>2.0062035387648947E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
+        <v>0.948445171849427</v>
+      </c>
+      <c r="C7">
         <v>0.95765139116202902</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>0.94352363413136897</v>
       </c>
-      <c r="D7">
-        <f>B7-C7</f>
+      <c r="E7">
+        <f t="shared" si="0"/>
         <v>1.4127757030660049E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
+        <v>0.94905891980360002</v>
+      </c>
+      <c r="C8">
         <v>0.95887888707037605</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>0.93799877225291595</v>
       </c>
-      <c r="D8">
-        <f>B8-C8</f>
+      <c r="E8">
+        <f t="shared" si="0"/>
         <v>2.0880114817460105E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
+        <v>0.94905891980360002</v>
+      </c>
+      <c r="C9">
         <v>0.95662847790507299</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>0.93861264579496595</v>
       </c>
-      <c r="D9">
-        <f>B9-C9</f>
+      <c r="E9">
+        <f t="shared" si="0"/>
         <v>1.8015832110107044E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
+        <v>0.95110474631751196</v>
+      </c>
+      <c r="C10">
         <v>0.95908346972176695</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>0.94782074892572099</v>
       </c>
-      <c r="D10">
-        <f>B10-C10</f>
+      <c r="E10">
+        <f t="shared" si="0"/>
         <v>1.1262720796045955E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
+        <v>0.95171849427168498</v>
+      </c>
+      <c r="C11">
         <v>0.96215220949263502</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>0.93922651933701595</v>
       </c>
-      <c r="D11">
-        <f>B11-C11</f>
+      <c r="E11">
+        <f t="shared" si="0"/>
         <v>2.2925690155619072E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
+        <v>0.95192307692307598</v>
+      </c>
+      <c r="C12">
         <v>0.96215220949263502</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>0.94045426642111696</v>
       </c>
-      <c r="D12">
-        <f>B12-C12</f>
+      <c r="E12">
+        <f t="shared" si="0"/>
         <v>2.1697943071518067E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
+        <v>0.95560556464811697</v>
+      </c>
+      <c r="C13">
         <v>0.95908346972176695</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>0.94290976058931797</v>
       </c>
-      <c r="D13">
-        <f>B13-C13</f>
+      <c r="E13">
+        <f t="shared" si="0"/>
         <v>1.6173709132448977E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
+        <v>0.95355973813420603</v>
+      </c>
+      <c r="C14">
         <v>0.96460720130932898</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>0.94229588704726797</v>
       </c>
-      <c r="D14">
-        <f>B14-C14</f>
+      <c r="E14">
+        <f t="shared" si="0"/>
         <v>2.2311314262061011E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>0.96624386252045802</v>
+        <v>0.95662847790507299</v>
       </c>
       <c r="C15">
-        <v>0.95273173726212401</v>
+        <v>0.965630114566284</v>
       </c>
       <c r="D15">
-        <f>B15-C15</f>
-        <v>1.3512125258334007E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+        <v>0.94597912829956998</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>1.9650986266714021E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
-        <v>0.95642389525368199</v>
+        <v>0.95130932896890297</v>
       </c>
       <c r="C16">
-        <v>0.94597912829956998</v>
+        <v>0.95458265139116205</v>
       </c>
       <c r="D16">
-        <f>B16-C16</f>
-        <v>1.0444766954112006E-2</v>
+        <v>0.94045426642111696</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>1.4128384970045094E-2</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -8479,248 +9010,252 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A16"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="3" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>0.96440261865793697</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>0.94597912829956998</v>
       </c>
-      <c r="D2">
-        <f>B2-C2</f>
+      <c r="E2">
+        <f t="shared" ref="E2:E16" si="0">C2-D2</f>
         <v>1.842349035836699E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>0.98240589198035999</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>0.97360343769183499</v>
       </c>
-      <c r="D3">
-        <f>B3-C3</f>
+      <c r="E3">
+        <f t="shared" si="0"/>
         <v>8.8024542885249968E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>0.99263502454991803</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>0.97912829957028802</v>
       </c>
-      <c r="D4">
-        <f>B4-C4</f>
+      <c r="E4">
+        <f t="shared" si="0"/>
         <v>1.3506724979630014E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>0.98915711947626805</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>0.97605893186003601</v>
       </c>
-      <c r="D5">
-        <f>B5-C5</f>
+      <c r="E5">
+        <f t="shared" si="0"/>
         <v>1.3098187616232049E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>0.99672667757774103</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>0.98096992019643903</v>
       </c>
-      <c r="D6">
-        <f>B6-C6</f>
+      <c r="E6">
+        <f t="shared" si="0"/>
         <v>1.5756757381302E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>0.99672667757774103</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>0.97974217311233802</v>
       </c>
-      <c r="D7">
-        <f>B7-C7</f>
+      <c r="E7">
+        <f t="shared" si="0"/>
         <v>1.6984504465403005E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>0.99836333878886996</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>0.97974217311233802</v>
       </c>
-      <c r="D8">
-        <f>B8-C8</f>
+      <c r="E8">
+        <f t="shared" si="0"/>
         <v>1.8621165676531937E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>0.99959083469721699</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>0.98342541436464004</v>
       </c>
-      <c r="D9">
-        <f>B9-C9</f>
+      <c r="E9">
+        <f t="shared" si="0"/>
         <v>1.6165420332576952E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>0.99774959083469705</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>0.98158379373848903</v>
       </c>
-      <c r="D10">
-        <f>B10-C10</f>
+      <c r="E10">
+        <f t="shared" si="0"/>
         <v>1.6165797096208023E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>0.99959083469721699</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>0.98158379373848903</v>
       </c>
-      <c r="D11">
-        <f>B11-C11</f>
+      <c r="E11">
+        <f t="shared" si="0"/>
         <v>1.800704095872796E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>0.99877250409165297</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>0.97851442602823802</v>
       </c>
-      <c r="D12">
-        <f>B12-C12</f>
+      <c r="E12">
+        <f t="shared" si="0"/>
         <v>2.0258078063414953E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>0.99877250409165297</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>0.97912829957028802</v>
       </c>
-      <c r="D13">
-        <f>B13-C13</f>
+      <c r="E13">
+        <f t="shared" si="0"/>
         <v>1.964420452136495E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="C14">
         <v>0.99959083469721699</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>0.97974217311233802</v>
       </c>
-      <c r="D14">
-        <f>B14-C14</f>
+      <c r="E14">
+        <f t="shared" si="0"/>
         <v>1.9848661584878968E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15">
+      <c r="C15">
         <v>0.99836333878886996</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>0.98035604665438902</v>
       </c>
-      <c r="D15">
-        <f>B15-C15</f>
+      <c r="E15">
+        <f t="shared" si="0"/>
         <v>1.8007292134480934E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16">
+      <c r="C16">
         <v>0.99324877250409105</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>0.97237569060773399</v>
       </c>
-      <c r="D16">
-        <f>B16-C16</f>
+      <c r="E16">
+        <f t="shared" si="0"/>
         <v>2.087308189635706E-2</v>
       </c>
     </row>
@@ -8732,247 +9267,251 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="3" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>0.98076923076922995</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>0.96992019643953298</v>
       </c>
-      <c r="D2">
-        <f>B2-C2</f>
+      <c r="E2">
+        <f t="shared" ref="E2:E16" si="0">C2-D2</f>
         <v>1.0849034329696972E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>0.99283960720130904</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>0.98096992019643903</v>
       </c>
-      <c r="D3">
-        <f>B3-C3</f>
+      <c r="E3">
+        <f t="shared" si="0"/>
         <v>1.1869687004870011E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>0.99836333878886996</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>0.98158379373848903</v>
       </c>
-      <c r="D4">
-        <f>B4-C4</f>
+      <c r="E4">
+        <f t="shared" si="0"/>
         <v>1.6779545050380928E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>0.99897708674304397</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>0.98465316144874104</v>
       </c>
-      <c r="D5">
-        <f>B5-C5</f>
+      <c r="E5">
+        <f t="shared" si="0"/>
         <v>1.432392529430293E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>0.999795417348608</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>0.98403928790669104</v>
       </c>
-      <c r="D6">
-        <f>B6-C6</f>
+      <c r="E6">
+        <f t="shared" si="0"/>
         <v>1.5756129441916955E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>0.99959083469721699</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>0.98403928790669104</v>
       </c>
-      <c r="D7">
-        <f>B7-C7</f>
+      <c r="E7">
+        <f t="shared" si="0"/>
         <v>1.555154679052595E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>1</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>0.98281154082259004</v>
       </c>
-      <c r="D8">
-        <f>B8-C8</f>
+      <c r="E8">
+        <f t="shared" si="0"/>
         <v>1.7188459177409965E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>1</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>0.98281154082259004</v>
       </c>
-      <c r="D9">
-        <f>B9-C9</f>
+      <c r="E9">
+        <f t="shared" si="0"/>
         <v>1.7188459177409965E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>1</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>0.98281154082259004</v>
       </c>
-      <c r="D10">
-        <f>B10-C10</f>
+      <c r="E10">
+        <f t="shared" si="0"/>
         <v>1.7188459177409965E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>1</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>0.98281154082259004</v>
       </c>
-      <c r="D11">
-        <f>B11-C11</f>
+      <c r="E11">
+        <f t="shared" si="0"/>
         <v>1.7188459177409965E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>1</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>0.98281154082259004</v>
       </c>
-      <c r="D12">
-        <f>B12-C12</f>
+      <c r="E12">
+        <f t="shared" si="0"/>
         <v>1.7188459177409965E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>1</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>0.98281154082259004</v>
       </c>
-      <c r="D13">
-        <f>B13-C13</f>
+      <c r="E13">
+        <f t="shared" si="0"/>
         <v>1.7188459177409965E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="C14">
         <v>1</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>0.98281154082259004</v>
       </c>
-      <c r="D14">
-        <f>B14-C14</f>
+      <c r="E14">
+        <f t="shared" si="0"/>
         <v>1.7188459177409965E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15">
+      <c r="C15">
         <v>1</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>0.98281154082259004</v>
       </c>
-      <c r="D15">
-        <f>B15-C15</f>
+      <c r="E15">
+        <f t="shared" si="0"/>
         <v>1.7188459177409965E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16">
+      <c r="C16">
         <v>1</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>0.98281154082259004</v>
       </c>
-      <c r="D16">
-        <f>B16-C16</f>
+      <c r="E16">
+        <f t="shared" si="0"/>
         <v>1.7188459177409965E-2</v>
       </c>
     </row>
@@ -8984,248 +9523,252 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C16"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="3" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>0.98792962356792102</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>0.96316758747697895</v>
       </c>
-      <c r="D2">
-        <f>B2-C2</f>
+      <c r="E2">
+        <f t="shared" ref="E2:E16" si="0">C2-D2</f>
         <v>2.4762036090942074E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>0.99611292962356701</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>0.97237569060773399</v>
       </c>
-      <c r="D3">
-        <f>B3-C3</f>
+      <c r="E3">
+        <f t="shared" si="0"/>
         <v>2.3737239015833023E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>0.99938625204582598</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>0.97728667894413701</v>
       </c>
-      <c r="D4">
-        <f>B4-C4</f>
+      <c r="E4">
+        <f t="shared" si="0"/>
         <v>2.2099573101688974E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>1</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>0.97728667894413701</v>
       </c>
-      <c r="D5">
-        <f>B5-C5</f>
+      <c r="E5">
+        <f t="shared" si="0"/>
         <v>2.2713321055862989E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>1</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>0.97728667894413701</v>
       </c>
-      <c r="D6">
-        <f>B6-C6</f>
+      <c r="E6">
+        <f t="shared" si="0"/>
         <v>2.2713321055862989E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>1</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>0.97728667894413701</v>
       </c>
-      <c r="D7">
-        <f>B7-C7</f>
+      <c r="E7">
+        <f t="shared" si="0"/>
         <v>2.2713321055862989E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>1</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>0.97728667894413701</v>
       </c>
-      <c r="D8">
-        <f>B8-C8</f>
+      <c r="E8">
+        <f t="shared" si="0"/>
         <v>2.2713321055862989E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>1</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>0.97728667894413701</v>
       </c>
-      <c r="D9">
-        <f>B9-C9</f>
+      <c r="E9">
+        <f t="shared" si="0"/>
         <v>2.2713321055862989E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>1</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>0.97728667894413701</v>
       </c>
-      <c r="D10">
-        <f>B10-C10</f>
+      <c r="E10">
+        <f t="shared" si="0"/>
         <v>2.2713321055862989E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>1</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>0.97728667894413701</v>
       </c>
-      <c r="D11">
-        <f>B11-C11</f>
+      <c r="E11">
+        <f t="shared" si="0"/>
         <v>2.2713321055862989E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>1</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>0.97728667894413701</v>
       </c>
-      <c r="D12">
-        <f>B12-C12</f>
+      <c r="E12">
+        <f t="shared" si="0"/>
         <v>2.2713321055862989E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>1</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>0.97728667894413701</v>
       </c>
-      <c r="D13">
-        <f>B13-C13</f>
+      <c r="E13">
+        <f t="shared" si="0"/>
         <v>2.2713321055862989E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="C14">
         <v>1</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>0.97728667894413701</v>
       </c>
-      <c r="D14">
-        <f>B14-C14</f>
+      <c r="E14">
+        <f t="shared" si="0"/>
         <v>2.2713321055862989E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15">
+      <c r="C15">
         <v>1</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>0.97728667894413701</v>
       </c>
-      <c r="D15">
-        <f>B15-C15</f>
+      <c r="E15">
+        <f t="shared" si="0"/>
         <v>2.2713321055862989E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16">
+      <c r="C16">
         <v>1</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>0.97728667894413701</v>
       </c>
-      <c r="D16">
-        <f>B16-C16</f>
+      <c r="E16">
+        <f t="shared" si="0"/>
         <v>2.2713321055862989E-2</v>
       </c>
     </row>
@@ -9237,254 +9780,259 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="3" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.90625" customWidth="1"/>
+    <col min="4" max="4" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>0.96706219312602204</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>0.949662369551872</v>
       </c>
-      <c r="D2">
-        <f>B2-C2</f>
+      <c r="E2">
+        <f t="shared" ref="E2:E16" si="0">C2-D2</f>
         <v>1.7399823574150042E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>0.99243044189852703</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>0.96439533456107995</v>
       </c>
-      <c r="D3">
-        <f>B3-C3</f>
+      <c r="E3">
+        <f t="shared" si="0"/>
         <v>2.8035107337447074E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>0.98936170212765895</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>0.96132596685082805</v>
       </c>
-      <c r="D4">
-        <f>B4-C4</f>
+      <c r="E4">
+        <f t="shared" si="0"/>
         <v>2.8035735276830898E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>0.99038461538461497</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>0.96500920810312996</v>
       </c>
-      <c r="D5">
-        <f>B5-C5</f>
+      <c r="E5">
+        <f t="shared" si="0"/>
         <v>2.5375407281485018E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>0.99754500818330605</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>0.96562308164518096</v>
       </c>
-      <c r="D6">
-        <f>B6-C6</f>
+      <c r="E6">
+        <f t="shared" si="0"/>
         <v>3.1921926538125089E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>0.99795417348608795</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>0.96562308164518096</v>
       </c>
-      <c r="D7">
-        <f>B7-C7</f>
+      <c r="E7">
+        <f t="shared" si="0"/>
         <v>3.2331091840906989E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>0.99856792144026096</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>0.96562308164518096</v>
       </c>
-      <c r="D8">
-        <f>B8-C8</f>
+      <c r="E8">
+        <f t="shared" si="0"/>
         <v>3.2944839795080005E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>0.99897708674304397</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>0.96562308164518096</v>
       </c>
-      <c r="D9">
-        <f>B9-C9</f>
+      <c r="E9">
+        <f t="shared" si="0"/>
         <v>3.3354005097863015E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>0.99897708674304397</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>0.96562308164518096</v>
       </c>
-      <c r="D10">
-        <f>B10-C10</f>
+      <c r="E10">
+        <f t="shared" si="0"/>
         <v>3.3354005097863015E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>0.99897708674304397</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>0.96562308164518096</v>
       </c>
-      <c r="D11">
-        <f>B11-C11</f>
+      <c r="E11">
+        <f t="shared" si="0"/>
         <v>3.3354005097863015E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>0.99918166939443498</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>0.96562308164518096</v>
       </c>
-      <c r="D12">
-        <f>B12-C12</f>
+      <c r="E12">
+        <f t="shared" si="0"/>
         <v>3.3558587749254021E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>0.99918166939443498</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>0.96562308164518096</v>
       </c>
-      <c r="D13">
-        <f>B13-C13</f>
+      <c r="E13">
+        <f t="shared" si="0"/>
         <v>3.3558587749254021E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="C14">
         <v>0.99938625204582598</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>0.96562308164518096</v>
       </c>
-      <c r="D14">
-        <f>B14-C14</f>
+      <c r="E14">
+        <f t="shared" si="0"/>
         <v>3.3763170400645026E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15">
+      <c r="C15">
         <v>0.99959083469721699</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>0.96562308164518096</v>
       </c>
-      <c r="D15">
-        <f>B15-C15</f>
+      <c r="E15">
+        <f t="shared" si="0"/>
         <v>3.3967753052036032E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16">
+      <c r="C16">
         <v>0.99959083469721699</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>0.96562308164518096</v>
       </c>
-      <c r="D16">
-        <f>B16-C16</f>
+      <c r="E16">
+        <f t="shared" si="0"/>
         <v>3.3967753052036032E-2</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Imp2 Report and Refine the code
</commit_message>
<xml_diff>
--- a/Assignment2/Report/report.xlsx
+++ b/Assignment2/Report/report.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310" tabRatio="724" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310" tabRatio="724"/>
   </bookViews>
   <sheets>
     <sheet name="GenPerceptron" sheetId="1" r:id="rId1"/>
@@ -383,11 +383,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1076859168"/>
-        <c:axId val="1075649952"/>
+        <c:axId val="589984576"/>
+        <c:axId val="812270976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1076859168"/>
+        <c:axId val="589984576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -430,7 +430,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1075649952"/>
+        <c:crossAx val="812270976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -438,7 +438,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1075649952"/>
+        <c:axId val="812270976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -489,7 +489,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1076859168"/>
+        <c:crossAx val="589984576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -845,11 +845,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1075653216"/>
-        <c:axId val="1292432128"/>
+        <c:axId val="812276960"/>
+        <c:axId val="812272064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1075653216"/>
+        <c:axId val="812276960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -892,7 +892,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1292432128"/>
+        <c:crossAx val="812272064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -900,7 +900,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1292432128"/>
+        <c:axId val="812272064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -951,7 +951,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1075653216"/>
+        <c:crossAx val="812276960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -965,6 +965,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1414,11 +1415,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1292434304"/>
-        <c:axId val="1292431584"/>
+        <c:axId val="812272608"/>
+        <c:axId val="812275872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1292434304"/>
+        <c:axId val="812272608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1461,7 +1462,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1292431584"/>
+        <c:crossAx val="812275872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1469,7 +1470,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1292431584"/>
+        <c:axId val="812275872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1520,7 +1521,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1292434304"/>
+        <c:crossAx val="812272608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1983,11 +1984,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1292432672"/>
-        <c:axId val="1292429408"/>
+        <c:axId val="812274784"/>
+        <c:axId val="812268256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1292432672"/>
+        <c:axId val="812274784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2030,7 +2031,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1292429408"/>
+        <c:crossAx val="812268256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2038,7 +2039,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1292429408"/>
+        <c:axId val="812268256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2089,7 +2090,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1292432672"/>
+        <c:crossAx val="812274784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2103,7 +2104,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2553,11 +2553,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1292431040"/>
-        <c:axId val="1292434848"/>
+        <c:axId val="812262816"/>
+        <c:axId val="812268800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1292431040"/>
+        <c:axId val="812262816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2600,7 +2600,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1292434848"/>
+        <c:crossAx val="812268800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2608,7 +2608,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1292434848"/>
+        <c:axId val="812268800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2659,7 +2659,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1292431040"/>
+        <c:crossAx val="812262816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2673,7 +2673,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3123,11 +3122,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1292435392"/>
-        <c:axId val="1292433216"/>
+        <c:axId val="812269888"/>
+        <c:axId val="812271520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1292435392"/>
+        <c:axId val="812269888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3170,7 +3169,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1292433216"/>
+        <c:crossAx val="812271520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3178,7 +3177,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1292433216"/>
+        <c:axId val="812271520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3229,7 +3228,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1292435392"/>
+        <c:crossAx val="812269888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3243,7 +3242,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3693,11 +3691,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1292433760"/>
-        <c:axId val="1292435936"/>
+        <c:axId val="812273696"/>
+        <c:axId val="812267712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1292433760"/>
+        <c:axId val="812273696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3740,7 +3738,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1292435936"/>
+        <c:crossAx val="812267712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3748,7 +3746,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1292435936"/>
+        <c:axId val="812267712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3799,7 +3797,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1292433760"/>
+        <c:crossAx val="812273696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8282,8 +8280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8585,7 +8583,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B2" sqref="B2:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10098,7 +10096,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>

</xml_diff>